<commit_message>
restored accuracy of the GUI
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -950,131 +950,131 @@
     </row>
     <row r="2" ht="100" customHeight="1">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\0001_001.jpg</t>
+          <t>GUI/Examples/human\00001_male_back.jpg</t>
         </is>
       </c>
     </row>
     <row r="3" ht="100" customHeight="1">
       <c r="A3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\0001_002.jpg</t>
+          <t>GUI/Examples/human\0001_001.jpg</t>
         </is>
       </c>
     </row>
     <row r="4" ht="100" customHeight="1">
       <c r="A4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\0001_003.jpg</t>
+          <t>GUI/Examples/human\0001_1_25004_107_32_106_221.jpeg</t>
         </is>
       </c>
     </row>
     <row r="5" ht="100" customHeight="1">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\0001_004.jpg</t>
+          <t>GUI/Examples/human\0001_a.png</t>
         </is>
       </c>
     </row>
     <row r="6" ht="100" customHeight="1">
       <c r="A6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="n">
         <v>1</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\0001_005.jpg</t>
+          <t>GUI/Examples/human\0_16.jpg</t>
         </is>
       </c>
     </row>
     <row r="7" ht="100" customHeight="1">
       <c r="A7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\0001_1_25004_107_32_106_221.jpeg</t>
+          <t>GUI/Examples/human\1_11.jpg</t>
         </is>
       </c>
     </row>
     <row r="8" ht="100" customHeight="1">
       <c r="A8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\0001_2_25023_116_134_128_330.jpeg</t>
+          <t>GUI/Examples/human\1_2.jpg</t>
         </is>
       </c>
     </row>
     <row r="9" ht="100" customHeight="1">
       <c r="A9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\0_16.jpg</t>
+          <t>GUI/Examples/human\1_28.jpg</t>
         </is>
       </c>
     </row>
     <row r="10" ht="100" customHeight="1">
       <c r="A10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10" t="n">
         <v>1</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\0_8.jpg</t>
+          <t>GUI/Examples/human\1_36.jpg</t>
         </is>
       </c>
     </row>
     <row r="11" ht="100" customHeight="1">
       <c r="A11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\1_2.jpg</t>
+          <t>GUI/Examples/human\1_52.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed GUI to have a dialogue box
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -957,7 +957,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\00001_male_back.jpg</t>
+          <t>Test_Examples/human\00001_male_back.jpg</t>
         </is>
       </c>
     </row>
@@ -970,7 +970,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\0001_001.jpg</t>
+          <t>Test_Examples/human\0001_001.jpg</t>
         </is>
       </c>
     </row>
@@ -983,7 +983,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\0001_1_25004_107_32_106_221.jpeg</t>
+          <t>Test_Examples/human\0001_1_25004_107_32_106_221.jpeg</t>
         </is>
       </c>
     </row>
@@ -996,7 +996,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\0001_a.png</t>
+          <t>Test_Examples/human\0001_a.png</t>
         </is>
       </c>
     </row>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\0_16.jpg</t>
+          <t>Test_Examples/human\0_16.jpg</t>
         </is>
       </c>
     </row>
@@ -1022,7 +1022,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\1_11.jpg</t>
+          <t>Test_Examples/human\1_11.jpg</t>
         </is>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\1_2.jpg</t>
+          <t>Test_Examples/human\1_2.jpg</t>
         </is>
       </c>
     </row>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\1_28.jpg</t>
+          <t>Test_Examples/human\1_28.jpg</t>
         </is>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\1_36.jpg</t>
+          <t>Test_Examples/human\1_36.jpg</t>
         </is>
       </c>
     </row>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>GUI/Examples/human\1_52.jpg</t>
+          <t>Test_Examples/human\1_52.jpg</t>
         </is>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>GUI/Examples/nonhuman\nonhuman_0.jpg</t>
+          <t>Test_Examples/nonhuman\nonhuman_0.jpg</t>
         </is>
       </c>
     </row>
@@ -1100,7 +1100,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>GUI/Examples/nonhuman\nonhuman_1.jpg</t>
+          <t>Test_Examples/nonhuman\nonhuman_1.jpg</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>GUI/Examples/nonhuman\nonhuman_2.jpg</t>
+          <t>Test_Examples/nonhuman\nonhuman_2.jpg</t>
         </is>
       </c>
     </row>
@@ -1126,7 +1126,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>GUI/Examples/nonhuman\nonhuman_3.jpg</t>
+          <t>Test_Examples/nonhuman\nonhuman_3.jpg</t>
         </is>
       </c>
     </row>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>GUI/Examples/nonhuman\nonhuman_4.jpg</t>
+          <t>Test_Examples/nonhuman\nonhuman_4.jpg</t>
         </is>
       </c>
     </row>
@@ -1152,7 +1152,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>GUI/Examples/nonhuman\nonhuman_5.jpg</t>
+          <t>Test_Examples/nonhuman\nonhuman_5.jpg</t>
         </is>
       </c>
     </row>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>GUI/Examples/nonhuman\nonhuman_6.jpg</t>
+          <t>Test_Examples/nonhuman\nonhuman_6.jpg</t>
         </is>
       </c>
     </row>
@@ -1178,7 +1178,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>GUI/Examples/nonhuman\nonhuman_7.jpg</t>
+          <t>Test_Examples/nonhuman\nonhuman_7.jpg</t>
         </is>
       </c>
     </row>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>GUI/Examples/nonhuman\nonhuman_8.jpg</t>
+          <t>Test_Examples/nonhuman\nonhuman_8.jpg</t>
         </is>
       </c>
     </row>
@@ -1204,7 +1204,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>GUI/Examples/nonhuman\nonhuman_9.jpg</t>
+          <t>Test_Examples/nonhuman\nonhuman_9.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>